<commit_message>
Remove external link from file
</commit_message>
<xml_diff>
--- a/InputData/land/PLANAbPiaSY/Potential Land Area Newly Affected by Pol in a Single Yr.xlsx
+++ b/InputData/land/PLANAbPiaSY/Potential Land Area Newly Affected by Pol in a Single Yr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\land\PLANAbPiaSY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CC6597-548D-41DD-B963-037E56DD9ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4FA273-33A9-47AA-BF70-EA38802D8C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,6 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId7"/>
-    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'TNC Data'!$A$3:$DW$51</definedName>
@@ -36,7 +35,7 @@
     <definedName name="grams_per_ton" localSheetId="1">#REF!</definedName>
     <definedName name="grams_per_ton">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1418,25 +1417,6 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="PLANAbPiaSY"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="4">
-          <cell r="B4">
-            <v>46881870</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1761,7 +1741,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20664,10 +20644,10 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21486,12 +21466,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <f>B4/[2]PLANAbPiaSY!$B$4</f>
-        <v>5.6695690679573998</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix to IRA land use settings
</commit_message>
<xml_diff>
--- a/InputData/land/PLANAbPiaSY/Potential Land Area Newly Affected by Pol in a Single Yr.xlsx
+++ b/InputData/land/PLANAbPiaSY/Potential Land Area Newly Affected by Pol in a Single Yr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\land\PLANAbPiaSY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\land\PLANAbPiaSY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1502825-F36D-4CA2-A1B9-AB1796547897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D57DA0-E230-4087-9E91-4A2E818FF32C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="386">
   <si>
     <t>PLANAbPiaSY Potential Land Area Newly Affected by Policy in a Single Year</t>
   </si>
@@ -1136,15 +1136,6 @@
     <t>Policy Settings:</t>
   </si>
   <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Moderate</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>Forest Management</t>
   </si>
   <si>
@@ -1256,13 +1247,13 @@
     <t>Afforestation and Reforestation Only</t>
   </si>
   <si>
-    <t>We phase in the expected forestry impacts so they reach their maximum in the year 2031, according to the following implementation schedule:</t>
-  </si>
-  <si>
     <t>We also adjust this variable to remove the potential implemented as part of Inflation Reduction Act</t>
   </si>
   <si>
     <t>calculations (see relevant tab for methodology).</t>
+  </si>
+  <si>
+    <t>We phase in the expected forestry impacts so they reach their maximum in the year 2032, according to the following implementation schedule:</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1532,7 @@
     <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1671,9 +1662,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1711,9 +1702,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1746,26 +1737,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1798,26 +1772,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1993,7 +1950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
@@ -2259,12 +2216,12 @@
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -22276,8 +22233,8 @@
   </sheetPr>
   <dimension ref="A1:BL86"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="K86" sqref="K86"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22444,57 +22401,41 @@
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A6" s="53"/>
-      <c r="B6" s="52" t="s">
-        <v>346</v>
-      </c>
-      <c r="C6" s="52" t="s">
-        <v>347</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>348</v>
-      </c>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
       <c r="G6" s="52"/>
       <c r="H6" s="54"/>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A7" s="53" t="s">
-        <v>349</v>
-      </c>
-      <c r="B7" s="52">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="C7" s="52">
-        <f t="shared" ref="C7:D8" si="0">B7</f>
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="D7" s="52">
-        <f t="shared" si="0"/>
-        <v>5.1999999999999998E-2</v>
-      </c>
+        <v>346</v>
+      </c>
+      <c r="B7" s="63">
+        <f>B62</f>
+        <v>4.7E-2</v>
+      </c>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
       <c r="G7" s="52"/>
       <c r="H7" s="54"/>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" s="53" t="s">
-        <v>350</v>
-      </c>
-      <c r="B8" s="52">
-        <v>0.37</v>
-      </c>
-      <c r="C8" s="52">
-        <f t="shared" si="0"/>
-        <v>0.37</v>
-      </c>
-      <c r="D8" s="52">
-        <f t="shared" si="0"/>
-        <v>0.37</v>
-      </c>
+        <v>347</v>
+      </c>
+      <c r="B8" s="64">
+        <f>B79</f>
+        <v>0.4</v>
+      </c>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
       <c r="G8" s="52"/>
       <c r="H8" s="54"/>
     </row>
     <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B9" s="53"/>
       <c r="C9" s="53"/>
@@ -22512,7 +22453,7 @@
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B11" s="54">
         <v>2020</v>
@@ -22521,7 +22462,7 @@
         <v>2022</v>
       </c>
       <c r="D11" s="54">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="E11" s="54">
         <v>2033</v>
@@ -22618,7 +22559,7 @@
     </row>
     <row r="14" spans="1:64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="53" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B14" s="54">
         <v>2020</v>
@@ -22627,10 +22568,10 @@
         <v>2022</v>
       </c>
       <c r="D14" s="54">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="E14" s="54">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="F14" s="54">
         <v>2050</v>
@@ -22902,7 +22843,7 @@
     </row>
     <row r="18" spans="1:64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="55" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B18" s="56">
         <f>SUM(B42:B43)*10^3/9</f>
@@ -23039,7 +22980,7 @@
     </row>
     <row r="20" spans="1:64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="55" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B20" s="54"/>
       <c r="C20" s="54"/>
@@ -23244,43 +23185,44 @@
         <v>0</v>
       </c>
       <c r="D22" s="58">
-        <f>1/9</f>
-        <v>0.1111111111111111</v>
+        <f>1/10</f>
+        <v>0.1</v>
       </c>
       <c r="E22" s="58">
-        <f t="shared" ref="E22:L22" si="1">D22+1/9</f>
-        <v>0.22222222222222221</v>
+        <f>D22+1/10</f>
+        <v>0.2</v>
       </c>
       <c r="F22" s="58">
-        <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
+        <f t="shared" ref="F22:M22" si="0">E22+1/10</f>
+        <v>0.30000000000000004</v>
       </c>
       <c r="G22" s="58">
-        <f t="shared" si="1"/>
-        <v>0.44444444444444442</v>
+        <f t="shared" si="0"/>
+        <v>0.4</v>
       </c>
       <c r="H22" s="58">
-        <f t="shared" si="1"/>
-        <v>0.55555555555555558</v>
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="I22" s="58">
-        <f t="shared" si="1"/>
-        <v>0.66666666666666674</v>
+        <f t="shared" si="0"/>
+        <v>0.6</v>
       </c>
       <c r="J22" s="58">
-        <f t="shared" si="1"/>
-        <v>0.7777777777777779</v>
+        <f t="shared" si="0"/>
+        <v>0.7</v>
       </c>
       <c r="K22" s="58">
-        <f t="shared" si="1"/>
-        <v>0.88888888888888906</v>
+        <f t="shared" si="0"/>
+        <v>0.79999999999999993</v>
       </c>
       <c r="L22" s="58">
-        <f t="shared" si="1"/>
-        <v>1.0000000000000002</v>
+        <f t="shared" si="0"/>
+        <v>0.89999999999999991</v>
       </c>
       <c r="M22" s="58">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.99999999999999989</v>
       </c>
       <c r="N22" s="58">
         <v>0</v>
@@ -23438,7 +23380,7 @@
     </row>
     <row r="24" spans="1:64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B24" s="49"/>
       <c r="C24" s="49"/>
@@ -23506,7 +23448,7 @@
     </row>
     <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A25" s="53" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B25" s="52">
         <v>0.78500000000000003</v>
@@ -23517,132 +23459,132 @@
     </row>
     <row r="27" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="28" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A28" s="57" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B28" s="54">
         <v>1.8</v>
       </c>
       <c r="C28" s="57"/>
       <c r="D28" s="57" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="29" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A29" s="57" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B29" s="54">
         <v>0.2</v>
       </c>
       <c r="C29" s="57"/>
       <c r="D29" s="57" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B30" s="54">
         <v>0.1</v>
       </c>
       <c r="C30" s="57"/>
       <c r="D30" s="57" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A31" s="57" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B31" s="54">
         <v>0.05</v>
       </c>
       <c r="C31" s="57"/>
       <c r="D31" s="57" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A32" s="57" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B32" s="54">
         <v>0.15</v>
       </c>
       <c r="C32" s="57"/>
       <c r="D32" s="57" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="33" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A33" s="57" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B33" s="54">
         <v>0.15</v>
       </c>
       <c r="C33" s="57"/>
       <c r="D33" s="57" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="34" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A34" s="57" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B34" s="54">
         <v>0.1</v>
       </c>
       <c r="C34" s="57"/>
       <c r="D34" s="57" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="35" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A35" s="57" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B35" s="54">
         <v>0.05</v>
       </c>
       <c r="C35" s="57"/>
       <c r="D35" s="57" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="36" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A36" s="57" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="B36" s="54">
         <v>0.1</v>
       </c>
       <c r="C36" s="57"/>
       <c r="D36" s="57" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="37" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A37" s="57" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B37" s="54">
         <v>0.7</v>
       </c>
       <c r="C37" s="57"/>
       <c r="D37" s="57" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="38" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A38" s="57" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B38" s="54">
         <v>1.5</v>
@@ -23654,25 +23596,25 @@
     </row>
     <row r="39" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A39" s="57" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B39" s="54">
         <v>0.1</v>
       </c>
       <c r="C39" s="57"/>
       <c r="D39" s="57" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="41" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A41" s="55" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B41" s="54"/>
     </row>
     <row r="42" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A42" s="57" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B42" s="54">
         <f>SUM(B31:B37)</f>
@@ -23690,7 +23632,7 @@
     </row>
     <row r="45" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="46" spans="1:64" x14ac:dyDescent="0.25">
@@ -23698,7 +23640,7 @@
     </row>
     <row r="47" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A47" s="53" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B47" s="52"/>
       <c r="C47" s="52"/>
@@ -23766,7 +23708,7 @@
     </row>
     <row r="48" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A48" s="52" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B48" s="52">
         <v>2020</v>
@@ -23896,7 +23838,7 @@
     </row>
     <row r="49" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A49" s="52" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B49" s="52">
         <v>0</v>
@@ -24026,7 +23968,7 @@
     </row>
     <row r="50" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A50" s="52" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B50" s="52">
         <v>0</v>
@@ -24156,7 +24098,7 @@
     </row>
     <row r="51" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A51" s="52" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B51" s="52">
         <v>0</v>
@@ -24286,7 +24228,7 @@
     </row>
     <row r="52" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A52" s="52" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B52" s="52">
         <v>0</v>
@@ -24416,7 +24358,7 @@
     </row>
     <row r="53" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A53" s="52" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B53" s="52">
         <v>0</v>
@@ -24546,7 +24488,7 @@
     </row>
     <row r="54" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A54" s="52" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B54" s="52">
         <v>0</v>
@@ -24676,7 +24618,7 @@
     </row>
     <row r="55" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A55" s="52" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B55" s="52">
         <v>0</v>
@@ -24806,7 +24748,7 @@
     </row>
     <row r="56" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A56" s="52" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B56" s="52">
         <v>0</v>
@@ -24936,7 +24878,7 @@
     </row>
     <row r="57" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A57" s="52" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B57" s="52">
         <v>0</v>
@@ -25066,7 +25008,7 @@
     </row>
     <row r="59" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A59" s="52" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B59" s="60">
         <f>B42*B25*10^9</f>
@@ -25075,7 +25017,7 @@
     </row>
     <row r="60" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A60" s="52" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B60" s="60">
         <f>SUM(E49:M51)</f>
@@ -25085,7 +25027,7 @@
     </row>
     <row r="62" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A62" s="52" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B62" s="61">
         <v>4.7E-2</v>
@@ -25159,7 +25101,7 @@
     </row>
     <row r="64" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A64" s="53" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B64" s="52"/>
       <c r="C64" s="52"/>
@@ -25227,7 +25169,7 @@
     </row>
     <row r="65" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A65" s="52" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B65" s="52">
         <v>2020</v>
@@ -25357,7 +25299,7 @@
     </row>
     <row r="66" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A66" s="52" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B66" s="52">
         <v>0</v>
@@ -25487,7 +25429,7 @@
     </row>
     <row r="67" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A67" s="52" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B67" s="52">
         <v>0</v>
@@ -25617,7 +25559,7 @@
     </row>
     <row r="68" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A68" s="52" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B68" s="52">
         <v>0</v>
@@ -25747,7 +25689,7 @@
     </row>
     <row r="69" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A69" s="52" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B69" s="52">
         <v>0</v>
@@ -25877,7 +25819,7 @@
     </row>
     <row r="70" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A70" s="52" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B70" s="52">
         <v>0</v>
@@ -26007,7 +25949,7 @@
     </row>
     <row r="71" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A71" s="52" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B71" s="52">
         <v>0</v>
@@ -26137,7 +26079,7 @@
     </row>
     <row r="72" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A72" s="52" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B72" s="52">
         <v>0</v>
@@ -26267,7 +26209,7 @@
     </row>
     <row r="73" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A73" s="52" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="B73" s="52">
         <v>0</v>
@@ -26397,7 +26339,7 @@
     </row>
     <row r="74" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A74" s="52" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B74" s="52">
         <v>0</v>
@@ -26527,7 +26469,7 @@
     </row>
     <row r="76" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A76" s="52" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="B76" s="60">
         <f>B43*B25*10^9</f>
@@ -26536,7 +26478,7 @@
     </row>
     <row r="77" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A77" s="52" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B77" s="60">
         <f>SUM(E66:M68)</f>
@@ -26545,7 +26487,7 @@
     </row>
     <row r="79" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A79" s="52" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="B79" s="62">
         <v>0.4</v>
@@ -26553,7 +26495,7 @@
     </row>
     <row r="81" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A81" s="53" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="82" spans="1:32" x14ac:dyDescent="0.25">
@@ -26656,7 +26598,7 @@
     </row>
     <row r="84" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -26668,52 +26610,56 @@
         <v>0</v>
       </c>
       <c r="E84" s="61">
-        <f>$M$84/9+D84</f>
-        <v>5.2222222222222218E-3</v>
+        <f>$N$84/10+D84</f>
+        <v>4.7000000000000002E-3</v>
       </c>
       <c r="F84" s="61">
-        <f t="shared" ref="F84:L84" si="2">$M$84/9+E84</f>
-        <v>1.0444444444444444E-2</v>
+        <f t="shared" ref="F84:M84" si="1">$N$84/10+E84</f>
+        <v>9.4000000000000004E-3</v>
       </c>
       <c r="G84" s="61">
-        <f t="shared" si="2"/>
-        <v>1.5666666666666666E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.4100000000000001E-2</v>
       </c>
       <c r="H84" s="61">
-        <f t="shared" si="2"/>
-        <v>2.0888888888888887E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.8800000000000001E-2</v>
       </c>
       <c r="I84" s="61">
-        <f t="shared" si="2"/>
-        <v>2.6111111111111109E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.35E-2</v>
       </c>
       <c r="J84" s="61">
-        <f t="shared" si="2"/>
-        <v>3.1333333333333331E-2</v>
+        <f t="shared" si="1"/>
+        <v>2.8199999999999999E-2</v>
       </c>
       <c r="K84" s="61">
-        <f t="shared" si="2"/>
-        <v>3.6555555555555549E-2</v>
+        <f t="shared" si="1"/>
+        <v>3.2899999999999999E-2</v>
       </c>
       <c r="L84" s="61">
-        <f t="shared" si="2"/>
-        <v>4.1777777777777775E-2</v>
-      </c>
-      <c r="M84" s="63">
+        <f t="shared" si="1"/>
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="M84" s="61">
+        <f t="shared" si="1"/>
+        <v>4.2300000000000004E-2</v>
+      </c>
+      <c r="N84" s="63">
         <f>B62</f>
         <v>4.7E-2</v>
       </c>
-      <c r="N84" s="60">
-        <v>0</v>
-      </c>
-      <c r="O84" s="60">
-        <v>0</v>
-      </c>
-      <c r="P84" s="60">
-        <v>0</v>
-      </c>
-      <c r="Q84" s="60">
-        <v>0</v>
+      <c r="O84" s="62">
+        <f>$N$84*0.75</f>
+        <v>3.5250000000000004E-2</v>
+      </c>
+      <c r="P84" s="62">
+        <f>N84*0.5</f>
+        <v>2.35E-2</v>
+      </c>
+      <c r="Q84" s="62">
+        <f>N84*0.25</f>
+        <v>1.175E-2</v>
       </c>
       <c r="R84" s="60">
         <v>0</v>
@@ -26775,55 +26721,52 @@
         <v>0</v>
       </c>
       <c r="E85" s="61">
-        <f>$M$85/9+D85</f>
-        <v>4.4444444444444446E-2</v>
+        <f>$N$85/10+D85</f>
+        <v>0.04</v>
       </c>
       <c r="F85" s="61">
-        <f t="shared" ref="F85:L85" si="3">$M$85/9+E85</f>
-        <v>8.8888888888888892E-2</v>
+        <f t="shared" ref="F85:M85" si="2">$N$85/10+E85</f>
+        <v>0.08</v>
       </c>
       <c r="G85" s="61">
-        <f t="shared" si="3"/>
-        <v>0.13333333333333333</v>
+        <f t="shared" si="2"/>
+        <v>0.12</v>
       </c>
       <c r="H85" s="61">
-        <f t="shared" si="3"/>
-        <v>0.17777777777777778</v>
+        <f t="shared" si="2"/>
+        <v>0.16</v>
       </c>
       <c r="I85" s="61">
-        <f t="shared" si="3"/>
-        <v>0.22222222222222224</v>
+        <f t="shared" si="2"/>
+        <v>0.2</v>
       </c>
       <c r="J85" s="61">
-        <f t="shared" si="3"/>
-        <v>0.26666666666666666</v>
+        <f t="shared" si="2"/>
+        <v>0.24000000000000002</v>
       </c>
       <c r="K85" s="61">
-        <f t="shared" si="3"/>
-        <v>0.31111111111111112</v>
+        <f t="shared" si="2"/>
+        <v>0.28000000000000003</v>
       </c>
       <c r="L85" s="61">
-        <f t="shared" si="3"/>
-        <v>0.35555555555555557</v>
-      </c>
-      <c r="M85" s="64">
+        <f t="shared" si="2"/>
+        <v>0.32</v>
+      </c>
+      <c r="M85" s="61">
+        <f t="shared" si="2"/>
+        <v>0.36</v>
+      </c>
+      <c r="N85" s="62">
         <f>B79</f>
         <v>0.4</v>
       </c>
-      <c r="N85" s="62">
-        <f>M85-$M$85/4</f>
-        <v>0.30000000000000004</v>
-      </c>
       <c r="O85" s="62">
-        <f t="shared" ref="O85:Q85" si="4">N85-$M$85/4</f>
-        <v>0.20000000000000004</v>
+        <v>0</v>
       </c>
       <c r="P85" s="62">
-        <f t="shared" si="4"/>
-        <v>0.10000000000000003</v>
+        <v>0</v>
       </c>
       <c r="Q85" s="62">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R85" s="60">
@@ -26914,117 +26857,114 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:AF7"/>
+  <dimension ref="A1:AE7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:AF1048576"/>
+      <selection activeCell="AD3" sqref="AD3:AE4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="32" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="31" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="2">
-        <v>2020</v>
-      </c>
-      <c r="C1">
+      <c r="B1">
         <v>2021</v>
       </c>
-      <c r="D1" s="2">
+      <c r="C1" s="2">
         <v>2022</v>
       </c>
-      <c r="E1">
+      <c r="D1">
         <v>2023</v>
       </c>
-      <c r="F1" s="2">
+      <c r="E1" s="2">
         <v>2024</v>
       </c>
-      <c r="G1">
+      <c r="F1">
         <v>2025</v>
       </c>
-      <c r="H1" s="2">
+      <c r="G1" s="2">
         <v>2026</v>
       </c>
-      <c r="I1">
+      <c r="H1">
         <v>2027</v>
       </c>
-      <c r="J1" s="2">
+      <c r="I1" s="2">
         <v>2028</v>
       </c>
-      <c r="K1">
+      <c r="J1">
         <v>2029</v>
       </c>
-      <c r="L1" s="2">
+      <c r="K1" s="2">
         <v>2030</v>
       </c>
-      <c r="M1">
+      <c r="L1">
         <v>2031</v>
       </c>
-      <c r="N1" s="2">
+      <c r="M1" s="2">
         <v>2032</v>
       </c>
-      <c r="O1">
+      <c r="N1">
         <v>2033</v>
       </c>
-      <c r="P1" s="2">
+      <c r="O1" s="2">
         <v>2034</v>
       </c>
-      <c r="Q1">
+      <c r="P1">
         <v>2035</v>
       </c>
-      <c r="R1" s="2">
+      <c r="Q1" s="2">
         <v>2036</v>
       </c>
-      <c r="S1">
+      <c r="R1">
         <v>2037</v>
       </c>
-      <c r="T1" s="2">
+      <c r="S1" s="2">
         <v>2038</v>
       </c>
-      <c r="U1">
+      <c r="T1">
         <v>2039</v>
       </c>
-      <c r="V1" s="2">
+      <c r="U1" s="2">
         <v>2040</v>
       </c>
-      <c r="W1">
+      <c r="V1">
         <v>2041</v>
       </c>
-      <c r="X1" s="2">
+      <c r="W1" s="2">
         <v>2042</v>
       </c>
-      <c r="Y1">
+      <c r="X1">
         <v>2043</v>
       </c>
-      <c r="Z1" s="2">
+      <c r="Y1" s="2">
         <v>2044</v>
       </c>
-      <c r="AA1">
+      <c r="Z1">
         <v>2045</v>
       </c>
-      <c r="AB1" s="2">
+      <c r="AA1" s="2">
         <v>2046</v>
       </c>
-      <c r="AC1">
+      <c r="AB1">
         <v>2047</v>
       </c>
-      <c r="AD1" s="2">
+      <c r="AC1" s="2">
         <v>2048</v>
       </c>
-      <c r="AE1">
+      <c r="AD1">
         <v>2049</v>
       </c>
-      <c r="AF1" s="2">
+      <c r="AE1" s="2">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -27148,270 +27088,258 @@
         <f>'Set Asides'!$A$29</f>
         <v>136290</v>
       </c>
-      <c r="AF2">
-        <f>'Set Asides'!$A$29</f>
-        <v>136290</v>
-      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!B85</f>
-        <v>3554041.2119197226</v>
-      </c>
-      <c r="C3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!C85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="D3" s="3">
+      <c r="C3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!D85</f>
         <v>3554041.2119197226</v>
       </c>
+      <c r="D3" s="3">
+        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!E85</f>
+        <v>3411879.5634429338</v>
+      </c>
       <c r="E3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!E85</f>
-        <v>3396083.8247232903</v>
+        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!F85</f>
+        <v>3269717.9149661446</v>
       </c>
       <c r="F3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!F85</f>
-        <v>3238126.4375268584</v>
+        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!G85</f>
+        <v>3127556.2664893558</v>
       </c>
       <c r="G3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!G85</f>
-        <v>3080169.0503304261</v>
+        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!H85</f>
+        <v>2985394.6180125671</v>
       </c>
       <c r="H3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!H85</f>
-        <v>2922211.6631339942</v>
+        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!I85</f>
+        <v>2843232.9695357783</v>
       </c>
       <c r="I3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!I85</f>
-        <v>2764254.2759375619</v>
+        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!J85</f>
+        <v>2701071.321058989</v>
       </c>
       <c r="J3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!J85</f>
-        <v>2606296.88874113</v>
+        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!K85</f>
+        <v>2558909.6725822003</v>
       </c>
       <c r="K3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!K85</f>
-        <v>2448339.5015446977</v>
+        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!L85</f>
+        <v>2416748.024105411</v>
       </c>
       <c r="L3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!L85</f>
-        <v>2290382.1143482653</v>
+        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!M85</f>
+        <v>2274586.3756286222</v>
       </c>
       <c r="M3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!M85</f>
+        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!N85</f>
         <v>2132424.7271518335</v>
       </c>
       <c r="N3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!N85</f>
-        <v>2487828.8483438054</v>
+        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!O85</f>
+        <v>3554041.2119197226</v>
       </c>
       <c r="O3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!O85</f>
-        <v>2843232.9695357778</v>
+        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!P85</f>
+        <v>3554041.2119197226</v>
       </c>
       <c r="P3" s="3">
-        <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!P85</f>
-        <v>3198637.0907277502</v>
-      </c>
-      <c r="Q3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!Q85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="R3" s="3">
+      <c r="Q3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!R85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="S3" s="3">
+      <c r="R3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!S85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="T3" s="3">
+      <c r="S3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!T85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="U3" s="3">
+      <c r="T3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!U85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="V3" s="3">
+      <c r="U3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!V85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="W3" s="3">
+      <c r="V3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!W85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="X3" s="3">
+      <c r="W3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!X85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="X3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!Y85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="Y3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!Z85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="Z3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!AA85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AA3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!AB85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AB3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!AC85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AC3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!AD85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="AE3" s="3">
+      <c r="AD3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!AE85</f>
         <v>3554041.2119197226</v>
       </c>
-      <c r="AF3" s="3">
+      <c r="AE3" s="3">
         <f>TNC_summary!$C$9-TNC_summary!$C$9*'Inflation Reduction Act'!AF85</f>
         <v>3554041.2119197226</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!B84</f>
-        <v>265800000</v>
-      </c>
-      <c r="C4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!C84</f>
         <v>265800000</v>
       </c>
-      <c r="D4" s="3">
+      <c r="C4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!D84</f>
         <v>265800000</v>
       </c>
+      <c r="D4" s="3">
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!E84</f>
+        <v>264550740</v>
+      </c>
       <c r="E4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!E84</f>
-        <v>264411933.33333334</v>
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!F84</f>
+        <v>263301480</v>
       </c>
       <c r="F4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!F84</f>
-        <v>263023866.66666666</v>
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!G84</f>
+        <v>262052220</v>
       </c>
       <c r="G4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!G84</f>
-        <v>261635800</v>
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!H84</f>
+        <v>260802960</v>
       </c>
       <c r="H4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!H84</f>
-        <v>260247733.33333334</v>
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!I84</f>
+        <v>259553700</v>
       </c>
       <c r="I4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!I84</f>
-        <v>258859666.66666666</v>
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!J84</f>
+        <v>258304440</v>
       </c>
       <c r="J4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!J84</f>
-        <v>257471600</v>
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!K84</f>
+        <v>257055180</v>
       </c>
       <c r="K4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!K84</f>
-        <v>256083533.33333334</v>
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!L84</f>
+        <v>255805920</v>
       </c>
       <c r="L4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!L84</f>
-        <v>254695466.66666666</v>
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!M84</f>
+        <v>254556660</v>
       </c>
       <c r="M4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!M84</f>
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!N84</f>
         <v>253307400</v>
       </c>
       <c r="N4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!N84</f>
-        <v>265800000</v>
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!O84</f>
+        <v>256430550</v>
       </c>
       <c r="O4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!O84</f>
-        <v>265800000</v>
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!P84</f>
+        <v>259553700</v>
       </c>
       <c r="P4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!P84</f>
-        <v>265800000</v>
+        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!Q84</f>
+        <v>262676850</v>
       </c>
       <c r="Q4" s="3">
-        <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!Q84</f>
-        <v>265800000</v>
-      </c>
-      <c r="R4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!R84</f>
         <v>265800000</v>
       </c>
-      <c r="S4" s="3">
+      <c r="R4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!S84</f>
         <v>265800000</v>
       </c>
-      <c r="T4" s="3">
+      <c r="S4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!T84</f>
         <v>265800000</v>
       </c>
-      <c r="U4" s="3">
+      <c r="T4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!U84</f>
         <v>265800000</v>
       </c>
-      <c r="V4" s="3">
+      <c r="U4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!V84</f>
         <v>265800000</v>
       </c>
-      <c r="W4" s="3">
+      <c r="V4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!W84</f>
         <v>265800000</v>
       </c>
-      <c r="X4" s="3">
+      <c r="W4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!X84</f>
         <v>265800000</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="X4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!Y84</f>
         <v>265800000</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="Y4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!Z84</f>
         <v>265800000</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="Z4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!AA84</f>
         <v>265800000</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AA4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!AB84</f>
         <v>265800000</v>
       </c>
-      <c r="AC4" s="3">
+      <c r="AB4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!AC84</f>
         <v>265800000</v>
       </c>
-      <c r="AD4" s="3">
+      <c r="AC4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!AD84</f>
         <v>265800000</v>
       </c>
-      <c r="AE4" s="3">
+      <c r="AD4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!AE84</f>
         <v>265800000</v>
       </c>
-      <c r="AF4" s="3">
+      <c r="AE4" s="3">
         <f>'Impr Forest Mgmt'!$A29-'Impr Forest Mgmt'!$A29*'Inflation Reduction Act'!AF84</f>
         <v>265800000</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -27535,20 +27463,17 @@
         <f>TNC_summary!$C$15</f>
         <v>187905.59808789165</v>
       </c>
-      <c r="AF5" s="3">
-        <f>TNC_summary!$C$15</f>
-        <v>187905.59808789165</v>
-      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>0</v>
+      <c r="C6" s="3">
+        <f>Peatland!$B$8</f>
+        <v>116927.89655172414</v>
       </c>
       <c r="D6" s="3">
         <f>Peatland!$B$8</f>
@@ -27662,12 +27587,8 @@
         <f>Peatland!$B$8</f>
         <v>116927.89655172414</v>
       </c>
-      <c r="AF6" s="3">
-        <f>Peatland!$B$8</f>
-        <v>116927.89655172414</v>
-      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -27788,10 +27709,6 @@
         <v>189275.41206509282</v>
       </c>
       <c r="AE7" s="3">
-        <f>TNC_summary!$C$20</f>
-        <v>189275.41206509282</v>
-      </c>
-      <c r="AF7" s="3">
         <f>TNC_summary!$C$20</f>
         <v>189275.41206509282</v>
       </c>

</xml_diff>